<commit_message>
Thu Sep 29 18:57:43 CST 2016
</commit_message>
<xml_diff>
--- a/netlist.xlsx
+++ b/netlist.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faster\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.54\share\web_news\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9075" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <t>http://www.itmsc.cn/category/list-313.html</t>
   </si>
   <si>
-    <t>http://tech.southcn.com/default.htm</t>
-  </si>
-  <si>
     <t>http://tech.sina.com.cn/</t>
   </si>
   <si>
@@ -192,12 +189,16 @@
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>http://www.southcn.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -235,6 +236,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -259,19 +267,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -551,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -578,7 +589,7 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -642,113 +653,116 @@
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" t="s">
+      <c r="A18" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>34</v>
+      <c r="A20" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A18" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Thu Sep 29 19:11:34 CST 2016
</commit_message>
<xml_diff>
--- a/netlist.xlsx
+++ b/netlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9075" tabRatio="990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>科学网</t>
   </si>
@@ -191,6 +191,10 @@
   </si>
   <si>
     <t>http://www.southcn.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>腾讯</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -560,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -724,31 +728,36 @@
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>